<commit_message>
include changes made at home
</commit_message>
<xml_diff>
--- a/raw-data/RSV Data.xlsx
+++ b/raw-data/RSV Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deborah/github/RSVcorrelates/raw-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAC2FE8-7368-A242-A306-9684F496D335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{376E60F2-2406-FB46-8243-E4AD5B610B0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5420" yWindow="1060" windowWidth="16800" windowHeight="18620" xr2:uid="{EB31B1D0-F9A6-424A-A571-FCA1CB7357B7}"/>
+    <workbookView xWindow="5420" yWindow="1060" windowWidth="24780" windowHeight="18620" activeTab="1" xr2:uid="{EB31B1D0-F9A6-424A-A571-FCA1CB7357B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,18 +18,8 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AC$71</definedName>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$W$60:$W$64</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$X$59</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$X$60:$X$64</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$Y$59</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$Y$60:$Y$64</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$W$60:$W$64</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$X$59</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$X$60:$X$64</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$Y$59</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$Y$60:$Y$64</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -50,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="76">
   <si>
     <t>Trial</t>
   </si>
@@ -266,6 +256,18 @@
   </si>
   <si>
     <t>JJ</t>
+  </si>
+  <si>
+    <t>Novavax</t>
+  </si>
+  <si>
+    <t>infants</t>
+  </si>
+  <si>
+    <t>mothers</t>
+  </si>
+  <si>
+    <t>elderly</t>
   </si>
 </sst>
 </file>
@@ -1791,10 +1793,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF8BCAD0-FE00-D14F-8109-AD4E81997C16}">
-  <dimension ref="A1:AC101"/>
+  <dimension ref="A1:AC137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="A98" activeCellId="1" sqref="A102:XFD102 A98:XFD98"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I133" sqref="I133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6406,6 +6409,1050 @@
         <v>11</v>
       </c>
     </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>72</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C102" t="s">
+        <v>39</v>
+      </c>
+      <c r="D102" t="s">
+        <v>72</v>
+      </c>
+      <c r="E102">
+        <v>0</v>
+      </c>
+      <c r="F102" t="s">
+        <v>8</v>
+      </c>
+      <c r="G102" t="s">
+        <v>48</v>
+      </c>
+      <c r="I102">
+        <v>763.59869174663402</v>
+      </c>
+      <c r="K102" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>72</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C103" t="s">
+        <v>39</v>
+      </c>
+      <c r="D103" t="s">
+        <v>72</v>
+      </c>
+      <c r="E103">
+        <v>0</v>
+      </c>
+      <c r="F103" t="s">
+        <v>9</v>
+      </c>
+      <c r="G103" t="s">
+        <v>48</v>
+      </c>
+      <c r="I103">
+        <v>678.89146677738302</v>
+      </c>
+      <c r="K103" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>72</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C104" t="s">
+        <v>39</v>
+      </c>
+      <c r="D104" t="s">
+        <v>72</v>
+      </c>
+      <c r="E104">
+        <v>14</v>
+      </c>
+      <c r="F104" t="s">
+        <v>9</v>
+      </c>
+      <c r="G104" t="s">
+        <v>48</v>
+      </c>
+      <c r="I104">
+        <v>457.294437414009</v>
+      </c>
+      <c r="K104" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>72</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C105" t="s">
+        <v>39</v>
+      </c>
+      <c r="D105" t="s">
+        <v>72</v>
+      </c>
+      <c r="E105">
+        <v>35</v>
+      </c>
+      <c r="F105" t="s">
+        <v>9</v>
+      </c>
+      <c r="G105" t="s">
+        <v>48</v>
+      </c>
+      <c r="I105">
+        <v>241.34239426132501</v>
+      </c>
+      <c r="K105" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>72</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C106" t="s">
+        <v>39</v>
+      </c>
+      <c r="D106" t="s">
+        <v>72</v>
+      </c>
+      <c r="E106">
+        <v>60</v>
+      </c>
+      <c r="F106" t="s">
+        <v>9</v>
+      </c>
+      <c r="G106" t="s">
+        <v>48</v>
+      </c>
+      <c r="I106">
+        <v>178.23938604266601</v>
+      </c>
+      <c r="K106" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>72</v>
+      </c>
+      <c r="B107" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C107" t="s">
+        <v>39</v>
+      </c>
+      <c r="D107" t="s">
+        <v>72</v>
+      </c>
+      <c r="E107">
+        <v>180</v>
+      </c>
+      <c r="F107" t="s">
+        <v>9</v>
+      </c>
+      <c r="G107" t="s">
+        <v>48</v>
+      </c>
+      <c r="I107">
+        <v>18.8677331449951</v>
+      </c>
+      <c r="K107" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>72</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C108" t="s">
+        <v>39</v>
+      </c>
+      <c r="D108" t="s">
+        <v>72</v>
+      </c>
+      <c r="E108">
+        <v>0</v>
+      </c>
+      <c r="F108" t="s">
+        <v>8</v>
+      </c>
+      <c r="G108" t="s">
+        <v>16</v>
+      </c>
+      <c r="I108">
+        <v>427.635276266728</v>
+      </c>
+      <c r="K108" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>72</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C109" t="s">
+        <v>39</v>
+      </c>
+      <c r="D109" t="s">
+        <v>72</v>
+      </c>
+      <c r="E109">
+        <v>0</v>
+      </c>
+      <c r="F109" t="s">
+        <v>9</v>
+      </c>
+      <c r="G109" t="s">
+        <v>16</v>
+      </c>
+      <c r="I109">
+        <v>513.982783488937</v>
+      </c>
+      <c r="K109" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>72</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C110" t="s">
+        <v>39</v>
+      </c>
+      <c r="D110" t="s">
+        <v>72</v>
+      </c>
+      <c r="E110">
+        <v>14</v>
+      </c>
+      <c r="F110" t="s">
+        <v>9</v>
+      </c>
+      <c r="G110" t="s">
+        <v>16</v>
+      </c>
+      <c r="I110">
+        <v>397.90770813353203</v>
+      </c>
+      <c r="K110" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>72</v>
+      </c>
+      <c r="B111" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C111" t="s">
+        <v>39</v>
+      </c>
+      <c r="D111" t="s">
+        <v>72</v>
+      </c>
+      <c r="E111">
+        <v>35</v>
+      </c>
+      <c r="F111" t="s">
+        <v>9</v>
+      </c>
+      <c r="G111" t="s">
+        <v>16</v>
+      </c>
+      <c r="I111">
+        <v>193.624809804059</v>
+      </c>
+      <c r="K111" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>72</v>
+      </c>
+      <c r="B112" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C112" t="s">
+        <v>39</v>
+      </c>
+      <c r="D112" t="s">
+        <v>72</v>
+      </c>
+      <c r="E112">
+        <v>60</v>
+      </c>
+      <c r="F112" t="s">
+        <v>9</v>
+      </c>
+      <c r="G112" t="s">
+        <v>16</v>
+      </c>
+      <c r="I112">
+        <v>95.292885618255198</v>
+      </c>
+      <c r="K112" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>72</v>
+      </c>
+      <c r="B113" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C113" t="s">
+        <v>39</v>
+      </c>
+      <c r="D113" t="s">
+        <v>72</v>
+      </c>
+      <c r="E113">
+        <v>180</v>
+      </c>
+      <c r="F113" t="s">
+        <v>9</v>
+      </c>
+      <c r="G113" t="s">
+        <v>16</v>
+      </c>
+      <c r="I113">
+        <v>16.417156709865498</v>
+      </c>
+      <c r="K113" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>72</v>
+      </c>
+      <c r="B114" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C114" t="s">
+        <v>39</v>
+      </c>
+      <c r="D114" t="s">
+        <v>72</v>
+      </c>
+      <c r="E114">
+        <v>0</v>
+      </c>
+      <c r="F114" t="s">
+        <v>8</v>
+      </c>
+      <c r="G114" t="s">
+        <v>48</v>
+      </c>
+      <c r="I114">
+        <v>476.410722979772</v>
+      </c>
+      <c r="K114" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>72</v>
+      </c>
+      <c r="B115" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C115" t="s">
+        <v>39</v>
+      </c>
+      <c r="D115" t="s">
+        <v>72</v>
+      </c>
+      <c r="E115">
+        <v>0</v>
+      </c>
+      <c r="F115" t="s">
+        <v>9</v>
+      </c>
+      <c r="G115" t="s">
+        <v>48</v>
+      </c>
+      <c r="I115">
+        <v>481.19275598334502</v>
+      </c>
+      <c r="K115" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>72</v>
+      </c>
+      <c r="B116" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C116" t="s">
+        <v>39</v>
+      </c>
+      <c r="D116" t="s">
+        <v>72</v>
+      </c>
+      <c r="E116">
+        <v>14</v>
+      </c>
+      <c r="F116" t="s">
+        <v>9</v>
+      </c>
+      <c r="G116" t="s">
+        <v>48</v>
+      </c>
+      <c r="I116">
+        <v>266.12203913594601</v>
+      </c>
+      <c r="K116" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>72</v>
+      </c>
+      <c r="B117" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C117" t="s">
+        <v>39</v>
+      </c>
+      <c r="D117" t="s">
+        <v>72</v>
+      </c>
+      <c r="E117">
+        <v>35</v>
+      </c>
+      <c r="F117" t="s">
+        <v>9</v>
+      </c>
+      <c r="G117" t="s">
+        <v>48</v>
+      </c>
+      <c r="I117">
+        <v>250.79947496044201</v>
+      </c>
+      <c r="K117" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>72</v>
+      </c>
+      <c r="B118" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C118" t="s">
+        <v>39</v>
+      </c>
+      <c r="D118" t="s">
+        <v>72</v>
+      </c>
+      <c r="E118">
+        <v>60</v>
+      </c>
+      <c r="F118" t="s">
+        <v>9</v>
+      </c>
+      <c r="G118" t="s">
+        <v>48</v>
+      </c>
+      <c r="I118">
+        <v>106.161851118908</v>
+      </c>
+      <c r="K118" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>72</v>
+      </c>
+      <c r="B119" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C119" t="s">
+        <v>39</v>
+      </c>
+      <c r="D119" t="s">
+        <v>72</v>
+      </c>
+      <c r="E119">
+        <v>180</v>
+      </c>
+      <c r="F119" t="s">
+        <v>9</v>
+      </c>
+      <c r="G119" t="s">
+        <v>48</v>
+      </c>
+      <c r="I119">
+        <v>21.2637039666409</v>
+      </c>
+      <c r="K119" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>72</v>
+      </c>
+      <c r="B120" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C120" t="s">
+        <v>39</v>
+      </c>
+      <c r="D120" t="s">
+        <v>72</v>
+      </c>
+      <c r="E120">
+        <v>0</v>
+      </c>
+      <c r="F120" t="s">
+        <v>8</v>
+      </c>
+      <c r="G120" t="s">
+        <v>16</v>
+      </c>
+      <c r="I120">
+        <v>414.53360810829298</v>
+      </c>
+      <c r="K120" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>72</v>
+      </c>
+      <c r="B121" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C121" t="s">
+        <v>39</v>
+      </c>
+      <c r="D121" t="s">
+        <v>72</v>
+      </c>
+      <c r="E121">
+        <v>0</v>
+      </c>
+      <c r="F121" t="s">
+        <v>9</v>
+      </c>
+      <c r="G121" t="s">
+        <v>16</v>
+      </c>
+      <c r="I121">
+        <v>470.16188037800902</v>
+      </c>
+      <c r="K121" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>72</v>
+      </c>
+      <c r="B122" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C122" t="s">
+        <v>39</v>
+      </c>
+      <c r="D122" t="s">
+        <v>72</v>
+      </c>
+      <c r="E122">
+        <v>14</v>
+      </c>
+      <c r="F122" t="s">
+        <v>9</v>
+      </c>
+      <c r="G122" t="s">
+        <v>16</v>
+      </c>
+      <c r="I122">
+        <v>343.46746089628903</v>
+      </c>
+      <c r="K122" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>72</v>
+      </c>
+      <c r="B123" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C123" t="s">
+        <v>39</v>
+      </c>
+      <c r="D123" t="s">
+        <v>72</v>
+      </c>
+      <c r="E123">
+        <v>35</v>
+      </c>
+      <c r="F123" t="s">
+        <v>9</v>
+      </c>
+      <c r="G123" t="s">
+        <v>16</v>
+      </c>
+      <c r="I123">
+        <v>220.770313619467</v>
+      </c>
+      <c r="K123" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>72</v>
+      </c>
+      <c r="B124" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C124" t="s">
+        <v>39</v>
+      </c>
+      <c r="D124" t="s">
+        <v>72</v>
+      </c>
+      <c r="E124">
+        <v>60</v>
+      </c>
+      <c r="F124" t="s">
+        <v>9</v>
+      </c>
+      <c r="G124" t="s">
+        <v>16</v>
+      </c>
+      <c r="I124">
+        <v>94.540602840280698</v>
+      </c>
+      <c r="K124" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>72</v>
+      </c>
+      <c r="B125" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C125" t="s">
+        <v>39</v>
+      </c>
+      <c r="D125" t="s">
+        <v>72</v>
+      </c>
+      <c r="E125">
+        <v>180</v>
+      </c>
+      <c r="F125" t="s">
+        <v>9</v>
+      </c>
+      <c r="G125" t="s">
+        <v>16</v>
+      </c>
+      <c r="I125">
+        <v>20.065951221747</v>
+      </c>
+      <c r="K125" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>72</v>
+      </c>
+      <c r="B126" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C126" t="s">
+        <v>39</v>
+      </c>
+      <c r="D126" t="s">
+        <v>72</v>
+      </c>
+      <c r="E126">
+        <v>0</v>
+      </c>
+      <c r="F126" t="s">
+        <v>8</v>
+      </c>
+      <c r="G126" t="s">
+        <v>48</v>
+      </c>
+      <c r="I126">
+        <v>266.55271718911098</v>
+      </c>
+      <c r="K126" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>72</v>
+      </c>
+      <c r="B127" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C127" t="s">
+        <v>39</v>
+      </c>
+      <c r="D127" t="s">
+        <v>72</v>
+      </c>
+      <c r="E127">
+        <v>28</v>
+      </c>
+      <c r="F127" t="s">
+        <v>8</v>
+      </c>
+      <c r="G127" t="s">
+        <v>48</v>
+      </c>
+      <c r="I127">
+        <v>509.94489548395501</v>
+      </c>
+      <c r="K127" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>72</v>
+      </c>
+      <c r="B128" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C128" t="s">
+        <v>39</v>
+      </c>
+      <c r="D128" t="s">
+        <v>72</v>
+      </c>
+      <c r="E128">
+        <v>56</v>
+      </c>
+      <c r="F128" t="s">
+        <v>8</v>
+      </c>
+      <c r="G128" t="s">
+        <v>48</v>
+      </c>
+      <c r="I128">
+        <v>480.475480592807</v>
+      </c>
+      <c r="K128" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>72</v>
+      </c>
+      <c r="B129" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C129" t="s">
+        <v>39</v>
+      </c>
+      <c r="D129" t="s">
+        <v>72</v>
+      </c>
+      <c r="E129">
+        <v>0</v>
+      </c>
+      <c r="F129" t="s">
+        <v>8</v>
+      </c>
+      <c r="G129" t="s">
+        <v>16</v>
+      </c>
+      <c r="I129">
+        <v>310.94578768440601</v>
+      </c>
+      <c r="K129" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>72</v>
+      </c>
+      <c r="B130" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C130" t="s">
+        <v>39</v>
+      </c>
+      <c r="D130" t="s">
+        <v>72</v>
+      </c>
+      <c r="E130">
+        <v>28</v>
+      </c>
+      <c r="F130" t="s">
+        <v>8</v>
+      </c>
+      <c r="G130" t="s">
+        <v>16</v>
+      </c>
+      <c r="I130">
+        <v>287.16081658929897</v>
+      </c>
+      <c r="K130" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>72</v>
+      </c>
+      <c r="B131" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C131" t="s">
+        <v>39</v>
+      </c>
+      <c r="D131" t="s">
+        <v>72</v>
+      </c>
+      <c r="E131">
+        <v>56</v>
+      </c>
+      <c r="F131" t="s">
+        <v>8</v>
+      </c>
+      <c r="G131" t="s">
+        <v>16</v>
+      </c>
+      <c r="I131">
+        <v>288.822523883504</v>
+      </c>
+      <c r="K131" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>72</v>
+      </c>
+      <c r="B132" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C132" t="s">
+        <v>39</v>
+      </c>
+      <c r="D132" t="s">
+        <v>72</v>
+      </c>
+      <c r="E132">
+        <v>0</v>
+      </c>
+      <c r="F132" t="s">
+        <v>8</v>
+      </c>
+      <c r="G132" t="s">
+        <v>48</v>
+      </c>
+      <c r="I132">
+        <v>274.88990968529299</v>
+      </c>
+      <c r="K132" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>72</v>
+      </c>
+      <c r="B133" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C133" t="s">
+        <v>39</v>
+      </c>
+      <c r="D133" t="s">
+        <v>72</v>
+      </c>
+      <c r="E133">
+        <v>28</v>
+      </c>
+      <c r="F133" t="s">
+        <v>8</v>
+      </c>
+      <c r="G133" t="s">
+        <v>48</v>
+      </c>
+      <c r="I133">
+        <v>669.92557424909899</v>
+      </c>
+      <c r="K133" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>72</v>
+      </c>
+      <c r="B134" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C134" t="s">
+        <v>39</v>
+      </c>
+      <c r="D134" t="s">
+        <v>72</v>
+      </c>
+      <c r="E134">
+        <v>56</v>
+      </c>
+      <c r="F134" t="s">
+        <v>8</v>
+      </c>
+      <c r="G134" t="s">
+        <v>48</v>
+      </c>
+      <c r="I134">
+        <v>591.73718510235801</v>
+      </c>
+      <c r="K134" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>72</v>
+      </c>
+      <c r="B135" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C135" t="s">
+        <v>39</v>
+      </c>
+      <c r="D135" t="s">
+        <v>72</v>
+      </c>
+      <c r="E135">
+        <v>0</v>
+      </c>
+      <c r="F135" t="s">
+        <v>8</v>
+      </c>
+      <c r="G135" t="s">
+        <v>16</v>
+      </c>
+      <c r="I135">
+        <v>223.99187806601799</v>
+      </c>
+      <c r="K135" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>72</v>
+      </c>
+      <c r="B136" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C136" t="s">
+        <v>39</v>
+      </c>
+      <c r="D136" t="s">
+        <v>72</v>
+      </c>
+      <c r="E136">
+        <v>28</v>
+      </c>
+      <c r="F136" t="s">
+        <v>8</v>
+      </c>
+      <c r="G136" t="s">
+        <v>16</v>
+      </c>
+      <c r="I136">
+        <v>236.16263440021001</v>
+      </c>
+      <c r="K136" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>72</v>
+      </c>
+      <c r="B137" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C137" t="s">
+        <v>39</v>
+      </c>
+      <c r="D137" t="s">
+        <v>72</v>
+      </c>
+      <c r="E137">
+        <v>56</v>
+      </c>
+      <c r="F137" t="s">
+        <v>8</v>
+      </c>
+      <c r="G137" t="s">
+        <v>16</v>
+      </c>
+      <c r="I137">
+        <v>240.06510841694799</v>
+      </c>
+      <c r="K137" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6414,10 +7461,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87136465-2DAE-EE48-9DCA-BA1E3F450528}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8:G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7010,6 +8058,230 @@
         <v>150</v>
       </c>
     </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" t="s">
+        <v>53</v>
+      </c>
+      <c r="G26">
+        <v>41.4</v>
+      </c>
+      <c r="H26">
+        <v>18</v>
+      </c>
+      <c r="I26">
+        <v>58.1</v>
+      </c>
+      <c r="J26" t="s">
+        <v>55</v>
+      </c>
+      <c r="K26">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" t="s">
+        <v>53</v>
+      </c>
+      <c r="G27">
+        <v>58.8</v>
+      </c>
+      <c r="H27">
+        <v>31.9</v>
+      </c>
+      <c r="I27">
+        <v>75</v>
+      </c>
+      <c r="J27" t="s">
+        <v>62</v>
+      </c>
+      <c r="K27">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" t="s">
+        <v>53</v>
+      </c>
+      <c r="G28">
+        <v>46.4</v>
+      </c>
+      <c r="H28">
+        <v>24.7</v>
+      </c>
+      <c r="I28">
+        <v>61.9</v>
+      </c>
+      <c r="J28" t="s">
+        <v>19</v>
+      </c>
+      <c r="K28">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" t="s">
+        <v>53</v>
+      </c>
+      <c r="E29">
+        <v>758</v>
+      </c>
+      <c r="F29">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30" t="s">
+        <v>53</v>
+      </c>
+      <c r="G30">
+        <v>12.6</v>
+      </c>
+      <c r="H30">
+        <v>-14</v>
+      </c>
+      <c r="I30">
+        <v>33</v>
+      </c>
+      <c r="J30" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" t="s">
+        <v>53</v>
+      </c>
+      <c r="G31">
+        <v>-7.9</v>
+      </c>
+      <c r="H31">
+        <v>-84</v>
+      </c>
+      <c r="I31">
+        <v>37</v>
+      </c>
+      <c r="J31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32" t="s">
+        <v>52</v>
+      </c>
+      <c r="D32" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32">
+        <v>509.94489548395501</v>
+      </c>
+      <c r="F32">
+        <v>310.94578768440601</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33">
+        <v>669.92557424909899</v>
+      </c>
+      <c r="F33">
+        <v>223.99187806601799</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="str">
+        <f>A33</f>
+        <v>Novavax</v>
+      </c>
+      <c r="B34" t="str">
+        <f>B33</f>
+        <v>Novavax</v>
+      </c>
+      <c r="C34" t="str">
+        <f>C33</f>
+        <v>Elderly</v>
+      </c>
+      <c r="D34" t="s">
+        <v>53</v>
+      </c>
+      <c r="E34">
+        <f>GEOMEAN(E32:E33)</f>
+        <v>584.48706310959983</v>
+      </c>
+      <c r="F34">
+        <f>GEOMEAN(F32:F33)</f>
+        <v>263.9115968655932</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
include more RSV studies
</commit_message>
<xml_diff>
--- a/raw-data/RSV Data.xlsx
+++ b/raw-data/RSV Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deborah/github/RSVcorrelates/raw-data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/z2211982/github/RSVcorrelates/raw-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{376E60F2-2406-FB46-8243-E4AD5B610B0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{373BAF05-92C7-8C41-8E4E-A1E6018AE09B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5420" yWindow="1060" windowWidth="24780" windowHeight="18620" activeTab="1" xr2:uid="{EB31B1D0-F9A6-424A-A571-FCA1CB7357B7}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1447" uniqueCount="87">
   <si>
     <t>Trial</t>
   </si>
@@ -269,6 +269,39 @@
   <si>
     <t>elderly</t>
   </si>
+  <si>
+    <t>GSK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arexvy </t>
+  </si>
+  <si>
+    <t>Moderna</t>
+  </si>
+  <si>
+    <t>MRNA-1345</t>
+  </si>
+  <si>
+    <t>MRNA-1346</t>
+  </si>
+  <si>
+    <t>MRNA-1347</t>
+  </si>
+  <si>
+    <t>MRNA-1348</t>
+  </si>
+  <si>
+    <t>MRNA-1349</t>
+  </si>
+  <si>
+    <t>Bavarian Nordic</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
 </sst>
 </file>
 
@@ -277,7 +310,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -288,6 +321,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1793,11 +1832,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF8BCAD0-FE00-D14F-8109-AD4E81997C16}">
-  <dimension ref="A1:AC137"/>
+  <dimension ref="A1:AC149"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I133" sqref="I133"/>
+      <pane ySplit="1" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I146" activeCellId="1" sqref="I144 I146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7453,6 +7492,354 @@
         <v>10</v>
       </c>
     </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>78</v>
+      </c>
+      <c r="B138" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C138" t="s">
+        <v>39</v>
+      </c>
+      <c r="D138" t="s">
+        <v>78</v>
+      </c>
+      <c r="E138">
+        <v>0</v>
+      </c>
+      <c r="F138" t="s">
+        <v>8</v>
+      </c>
+      <c r="G138" t="s">
+        <v>16</v>
+      </c>
+      <c r="I138">
+        <v>1377.5604903874701</v>
+      </c>
+      <c r="K138" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>78</v>
+      </c>
+      <c r="B139" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C139" t="s">
+        <v>39</v>
+      </c>
+      <c r="D139" t="s">
+        <v>78</v>
+      </c>
+      <c r="E139">
+        <v>0</v>
+      </c>
+      <c r="F139" t="s">
+        <v>8</v>
+      </c>
+      <c r="G139" t="s">
+        <v>48</v>
+      </c>
+      <c r="I139">
+        <v>1153.9516206390899</v>
+      </c>
+      <c r="K139" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>78</v>
+      </c>
+      <c r="B140" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C140" t="s">
+        <v>39</v>
+      </c>
+      <c r="D140" t="s">
+        <v>78</v>
+      </c>
+      <c r="E140">
+        <v>30</v>
+      </c>
+      <c r="F140" t="s">
+        <v>8</v>
+      </c>
+      <c r="G140" t="s">
+        <v>48</v>
+      </c>
+      <c r="I140">
+        <v>13325.998891345</v>
+      </c>
+      <c r="K140" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>78</v>
+      </c>
+      <c r="B141" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C141" t="s">
+        <v>39</v>
+      </c>
+      <c r="D141" t="s">
+        <v>78</v>
+      </c>
+      <c r="E141">
+        <v>60</v>
+      </c>
+      <c r="F141" t="s">
+        <v>8</v>
+      </c>
+      <c r="G141" t="s">
+        <v>48</v>
+      </c>
+      <c r="I141">
+        <v>10419.607195087199</v>
+      </c>
+      <c r="K141" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>78</v>
+      </c>
+      <c r="B142" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C142" t="s">
+        <v>39</v>
+      </c>
+      <c r="D142" t="s">
+        <v>78</v>
+      </c>
+      <c r="E142">
+        <v>90</v>
+      </c>
+      <c r="F142" t="s">
+        <v>8</v>
+      </c>
+      <c r="G142" t="s">
+        <v>48</v>
+      </c>
+      <c r="I142">
+        <v>8746.5556943389493</v>
+      </c>
+      <c r="K142" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>78</v>
+      </c>
+      <c r="B143" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C143" t="s">
+        <v>39</v>
+      </c>
+      <c r="D143" t="s">
+        <v>78</v>
+      </c>
+      <c r="E143">
+        <v>180</v>
+      </c>
+      <c r="F143" t="s">
+        <v>8</v>
+      </c>
+      <c r="G143" t="s">
+        <v>48</v>
+      </c>
+      <c r="I143">
+        <v>5729.6814462350803</v>
+      </c>
+      <c r="K143" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>78</v>
+      </c>
+      <c r="B144" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C144" t="s">
+        <v>39</v>
+      </c>
+      <c r="D144" t="s">
+        <v>78</v>
+      </c>
+      <c r="E144">
+        <v>0</v>
+      </c>
+      <c r="F144" t="s">
+        <v>8</v>
+      </c>
+      <c r="G144" t="s">
+        <v>16</v>
+      </c>
+      <c r="I144">
+        <v>2113.6892331321401</v>
+      </c>
+      <c r="K144" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>78</v>
+      </c>
+      <c r="B145" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C145" t="s">
+        <v>39</v>
+      </c>
+      <c r="D145" t="s">
+        <v>78</v>
+      </c>
+      <c r="E145">
+        <v>0</v>
+      </c>
+      <c r="F145" t="s">
+        <v>8</v>
+      </c>
+      <c r="G145" t="s">
+        <v>48</v>
+      </c>
+      <c r="I145">
+        <v>1647.6610012426499</v>
+      </c>
+      <c r="K145" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>78</v>
+      </c>
+      <c r="B146" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C146" t="s">
+        <v>39</v>
+      </c>
+      <c r="D146" t="s">
+        <v>78</v>
+      </c>
+      <c r="E146">
+        <v>30</v>
+      </c>
+      <c r="F146" t="s">
+        <v>8</v>
+      </c>
+      <c r="G146" t="s">
+        <v>48</v>
+      </c>
+      <c r="I146">
+        <v>13947.175264341</v>
+      </c>
+      <c r="K146" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>78</v>
+      </c>
+      <c r="B147" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C147" t="s">
+        <v>39</v>
+      </c>
+      <c r="D147" t="s">
+        <v>78</v>
+      </c>
+      <c r="E147">
+        <v>60</v>
+      </c>
+      <c r="F147" t="s">
+        <v>8</v>
+      </c>
+      <c r="G147" t="s">
+        <v>48</v>
+      </c>
+      <c r="I147">
+        <v>11698.0459051707</v>
+      </c>
+      <c r="K147" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>78</v>
+      </c>
+      <c r="B148" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C148" t="s">
+        <v>39</v>
+      </c>
+      <c r="D148" t="s">
+        <v>78</v>
+      </c>
+      <c r="E148">
+        <v>90</v>
+      </c>
+      <c r="F148" t="s">
+        <v>8</v>
+      </c>
+      <c r="G148" t="s">
+        <v>48</v>
+      </c>
+      <c r="I148">
+        <v>9470.2519508610403</v>
+      </c>
+      <c r="K148" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>78</v>
+      </c>
+      <c r="B149" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C149" t="s">
+        <v>39</v>
+      </c>
+      <c r="D149" t="s">
+        <v>78</v>
+      </c>
+      <c r="E149">
+        <v>180</v>
+      </c>
+      <c r="F149" t="s">
+        <v>8</v>
+      </c>
+      <c r="G149" t="s">
+        <v>48</v>
+      </c>
+      <c r="I149">
+        <v>7944.2656978701298</v>
+      </c>
+      <c r="K149" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7461,11 +7848,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87136465-2DAE-EE48-9DCA-BA1E3F450528}">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F34" sqref="F34"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J47" sqref="J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8237,7 +8624,7 @@
         <v>310.94578768440601</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>72</v>
       </c>
@@ -8257,7 +8644,7 @@
         <v>223.99187806601799</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="str">
         <f>A33</f>
         <v>Novavax</v>
@@ -8282,7 +8669,394 @@
         <v>263.9115968655932</v>
       </c>
     </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35" t="s">
+        <v>77</v>
+      </c>
+      <c r="C35" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" t="s">
+        <v>53</v>
+      </c>
+      <c r="G35">
+        <v>82.6</v>
+      </c>
+      <c r="H35">
+        <v>57.9</v>
+      </c>
+      <c r="I35">
+        <v>94.1</v>
+      </c>
+      <c r="J35" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>76</v>
+      </c>
+      <c r="B36" t="s">
+        <v>77</v>
+      </c>
+      <c r="C36" t="s">
+        <v>52</v>
+      </c>
+      <c r="D36" t="s">
+        <v>53</v>
+      </c>
+      <c r="G36">
+        <v>94.1</v>
+      </c>
+      <c r="H36">
+        <v>62.4</v>
+      </c>
+      <c r="I36">
+        <v>99.9</v>
+      </c>
+      <c r="J36" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>76</v>
+      </c>
+      <c r="B37" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" t="s">
+        <v>52</v>
+      </c>
+      <c r="D37" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37">
+        <v>9329.7000000000007</v>
+      </c>
+      <c r="F37">
+        <v>928.6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38" t="s">
+        <v>77</v>
+      </c>
+      <c r="C38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D38" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38">
+        <v>10178.9</v>
+      </c>
+      <c r="F38">
+        <v>1124.0999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39" t="s">
+        <v>52</v>
+      </c>
+      <c r="D39" t="s">
+        <v>53</v>
+      </c>
+      <c r="E39">
+        <f>GEOMEAN(E37:E38)</f>
+        <v>9745.0543010288038</v>
+      </c>
+      <c r="F39">
+        <f>GEOMEAN(F37:F38)</f>
+        <v>1021.6845207792862</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" t="s">
+        <v>79</v>
+      </c>
+      <c r="C40" t="s">
+        <v>52</v>
+      </c>
+      <c r="D40" t="s">
+        <v>53</v>
+      </c>
+      <c r="G40">
+        <v>83.7</v>
+      </c>
+      <c r="H40">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="I40">
+        <v>92.2</v>
+      </c>
+      <c r="J40" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41" t="s">
+        <v>80</v>
+      </c>
+      <c r="C41" t="s">
+        <v>52</v>
+      </c>
+      <c r="D41" t="s">
+        <v>53</v>
+      </c>
+      <c r="G41">
+        <v>82.4</v>
+      </c>
+      <c r="H41">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="I41">
+        <v>95.3</v>
+      </c>
+      <c r="J41" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>78</v>
+      </c>
+      <c r="B42" t="s">
+        <v>81</v>
+      </c>
+      <c r="C42" t="s">
+        <v>52</v>
+      </c>
+      <c r="D42" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42">
+        <v>13325.998891345</v>
+      </c>
+      <c r="F42">
+        <v>1377.5604903874701</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>78</v>
+      </c>
+      <c r="B43" t="s">
+        <v>82</v>
+      </c>
+      <c r="C43" t="s">
+        <v>52</v>
+      </c>
+      <c r="D43" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43">
+        <v>13947.175264341</v>
+      </c>
+      <c r="F43">
+        <v>2113.6892331321401</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>78</v>
+      </c>
+      <c r="B44" t="s">
+        <v>83</v>
+      </c>
+      <c r="C44" t="s">
+        <v>52</v>
+      </c>
+      <c r="D44" t="s">
+        <v>53</v>
+      </c>
+      <c r="E44">
+        <f>GEOMEAN(E42:E43)</f>
+        <v>13633.049626184253</v>
+      </c>
+      <c r="F44">
+        <f>GEOMEAN(F42:F43)</f>
+        <v>1706.38060716835</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>84</v>
+      </c>
+      <c r="C45" t="s">
+        <v>52</v>
+      </c>
+      <c r="D45" t="s">
+        <v>53</v>
+      </c>
+      <c r="G45">
+        <v>59</v>
+      </c>
+      <c r="J45" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>84</v>
+      </c>
+      <c r="C46" t="s">
+        <v>52</v>
+      </c>
+      <c r="D46" t="s">
+        <v>53</v>
+      </c>
+      <c r="G46">
+        <v>42.9</v>
+      </c>
+      <c r="J46" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>84</v>
+      </c>
+      <c r="B47" t="s">
+        <v>85</v>
+      </c>
+      <c r="C47" t="s">
+        <v>52</v>
+      </c>
+      <c r="D47" t="s">
+        <v>10</v>
+      </c>
+      <c r="E47">
+        <v>316.7</v>
+      </c>
+      <c r="F47">
+        <v>251.7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>84</v>
+      </c>
+      <c r="B48" t="s">
+        <v>85</v>
+      </c>
+      <c r="C48" t="s">
+        <v>52</v>
+      </c>
+      <c r="D48" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48">
+        <v>517.70000000000005</v>
+      </c>
+      <c r="F48">
+        <v>477.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>84</v>
+      </c>
+      <c r="B49" t="s">
+        <v>86</v>
+      </c>
+      <c r="C49" t="s">
+        <v>52</v>
+      </c>
+      <c r="D49" t="s">
+        <v>10</v>
+      </c>
+      <c r="E49">
+        <v>356.9</v>
+      </c>
+      <c r="F49">
+        <v>251.7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>84</v>
+      </c>
+      <c r="B50" t="s">
+        <v>86</v>
+      </c>
+      <c r="C50" t="s">
+        <v>52</v>
+      </c>
+      <c r="D50" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50">
+        <v>688.6</v>
+      </c>
+      <c r="F50">
+        <v>477.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>84</v>
+      </c>
+      <c r="B51" t="s">
+        <v>85</v>
+      </c>
+      <c r="C51" t="s">
+        <v>52</v>
+      </c>
+      <c r="D51" t="s">
+        <v>53</v>
+      </c>
+      <c r="E51">
+        <f>GEOMEAN(E47:E48)</f>
+        <v>404.91429957461366</v>
+      </c>
+      <c r="F51">
+        <f>GEOMEAN(F47:F48)</f>
+        <v>346.67960713027236</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>84</v>
+      </c>
+      <c r="B52" t="s">
+        <v>86</v>
+      </c>
+      <c r="C52" t="s">
+        <v>52</v>
+      </c>
+      <c r="D52" t="s">
+        <v>53</v>
+      </c>
+      <c r="E52">
+        <f>GEOMEAN(E49:E50)</f>
+        <v>495.74321982252059</v>
+      </c>
+      <c r="F52">
+        <f>GEOMEAN(F49:F50)</f>
+        <v>346.67960713027236</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
include two new papers
</commit_message>
<xml_diff>
--- a/raw-data/RSV Data.xlsx
+++ b/raw-data/RSV Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deborah/github/RSVcorrelates/raw-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{376E60F2-2406-FB46-8243-E4AD5B610B0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFEA9F46-8FDB-F645-BF4B-DF736037BE1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5420" yWindow="1060" windowWidth="24780" windowHeight="18620" activeTab="1" xr2:uid="{EB31B1D0-F9A6-424A-A571-FCA1CB7357B7}"/>
   </bookViews>
@@ -18,6 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AC$71</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$O$48</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1407" uniqueCount="94">
   <si>
     <t>Trial</t>
   </si>
@@ -268,6 +269,60 @@
   </si>
   <si>
     <t>elderly</t>
+  </si>
+  <si>
+    <t>Note these are numbers from table 3 that are different to the sticker price numbers</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Drug name</t>
+  </si>
+  <si>
+    <t>Nirsevimab</t>
+  </si>
+  <si>
+    <t>HARMONIE</t>
+  </si>
+  <si>
+    <t>mRNA-1345</t>
+  </si>
+  <si>
+    <t>Paper</t>
+  </si>
+  <si>
+    <t>https://www.nejm.org/doi/full/10.1056/NEJMoa2110275</t>
+  </si>
+  <si>
+    <t>https://www.nejm.org/doi/full/10.1056/NEJMoa2309189</t>
+  </si>
+  <si>
+    <t>https://www.nejm.org/doi/pdf/10.1056/NEJMoa2307079</t>
+  </si>
+  <si>
+    <t>Moderna</t>
+  </si>
+  <si>
+    <t>3 signs / symptoms</t>
+  </si>
+  <si>
+    <t>2 signs / symptoms</t>
+  </si>
+  <si>
+    <t>acute</t>
+  </si>
+  <si>
+    <t>ConquerRSV</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC9752082/pdf/ofac492.312.pdf</t>
+  </si>
+  <si>
+    <t>YoungAdults</t>
+  </si>
+  <si>
+    <t>These are actually very severe</t>
   </si>
 </sst>
 </file>
@@ -1796,7 +1851,7 @@
   <dimension ref="A1:AC137"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I133" sqref="I133"/>
     </sheetView>
   </sheetViews>
@@ -7461,11 +7516,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87136465-2DAE-EE48-9DCA-BA1E3F450528}">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:N49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F34" sqref="F34"/>
+      <selection pane="bottomLeft" activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7474,7 +7529,7 @@
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>69</v>
       </c>
@@ -7508,8 +7563,17 @@
       <c r="K1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L1" t="s">
+        <v>78</v>
+      </c>
+      <c r="M1" t="s">
+        <v>77</v>
+      </c>
+      <c r="N1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -7526,7 +7590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -7543,7 +7607,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -7562,7 +7626,7 @@
         <v>0.94868329805051377</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>51</v>
       </c>
@@ -7588,7 +7652,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -7611,7 +7675,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -7634,7 +7698,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -7654,7 +7718,7 @@
         <v>2121.2885444118601</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -7674,7 +7738,7 @@
         <v>2241.7131332343301</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -7694,7 +7758,7 @@
         <v>1978.45283958037</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -7716,7 +7780,7 @@
         <v>2105.9733412301466</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -7742,7 +7806,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -7768,7 +7832,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -7785,7 +7849,7 @@
         <v>2076</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -7802,7 +7866,7 @@
         <v>1763.6618147382401</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -7821,7 +7885,7 @@
         <v>1913.4685592913688</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -7848,7 +7912,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -7875,7 +7939,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -7902,7 +7966,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>63</v>
       </c>
@@ -7921,8 +7985,11 @@
       <c r="F20">
         <v>61.578757462956801</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>63</v>
       </c>
@@ -7941,8 +8008,11 @@
       <c r="F21">
         <v>84.659329584062505</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>63</v>
       </c>
@@ -7970,8 +8040,11 @@
       <c r="K22">
         <v>150</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>63</v>
       </c>
@@ -7999,8 +8072,11 @@
       <c r="K23">
         <v>150</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>63</v>
       </c>
@@ -8028,8 +8104,17 @@
       <c r="K24">
         <v>150</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L24" t="s">
+        <v>79</v>
+      </c>
+      <c r="M24" t="s">
+        <v>76</v>
+      </c>
+      <c r="N24" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>63</v>
       </c>
@@ -8057,13 +8142,22 @@
       <c r="K25">
         <v>150</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L25" t="s">
+        <v>79</v>
+      </c>
+      <c r="M25" t="s">
+        <v>76</v>
+      </c>
+      <c r="N25" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B26" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="C26" t="s">
         <v>61</v>
@@ -8072,27 +8166,33 @@
         <v>53</v>
       </c>
       <c r="G26">
-        <v>41.4</v>
+        <v>83.2</v>
       </c>
       <c r="H26">
-        <v>18</v>
+        <v>67.8</v>
       </c>
       <c r="I26">
-        <v>58.1</v>
+        <v>92</v>
       </c>
       <c r="J26" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="K26">
         <v>90</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L26" t="s">
+        <v>79</v>
+      </c>
+      <c r="N26" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B27" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="C27" t="s">
         <v>61</v>
@@ -8101,22 +8201,31 @@
         <v>53</v>
       </c>
       <c r="G27">
-        <v>58.8</v>
+        <v>75.7</v>
       </c>
       <c r="H27">
-        <v>31.9</v>
+        <v>32.799999999999997</v>
       </c>
       <c r="I27">
-        <v>75</v>
+        <v>92.9</v>
       </c>
       <c r="J27" t="s">
-        <v>62</v>
+        <v>19</v>
       </c>
       <c r="K27">
         <v>90</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L27" t="s">
+        <v>79</v>
+      </c>
+      <c r="M27" t="s">
+        <v>93</v>
+      </c>
+      <c r="N27" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>72</v>
       </c>
@@ -8130,22 +8239,22 @@
         <v>53</v>
       </c>
       <c r="G28">
-        <v>46.4</v>
+        <v>41.4</v>
       </c>
       <c r="H28">
-        <v>24.7</v>
+        <v>18</v>
       </c>
       <c r="I28">
-        <v>61.9</v>
+        <v>58.1</v>
       </c>
       <c r="J28" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="K28">
         <v>90</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>72</v>
       </c>
@@ -8158,14 +8267,23 @@
       <c r="D29" t="s">
         <v>53</v>
       </c>
-      <c r="E29">
-        <v>758</v>
-      </c>
-      <c r="F29">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G29">
+        <v>58.8</v>
+      </c>
+      <c r="H29">
+        <v>31.9</v>
+      </c>
+      <c r="I29">
+        <v>75</v>
+      </c>
+      <c r="J29" t="s">
+        <v>62</v>
+      </c>
+      <c r="K29">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>72</v>
       </c>
@@ -8173,25 +8291,28 @@
         <v>72</v>
       </c>
       <c r="C30" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="D30" t="s">
         <v>53</v>
       </c>
       <c r="G30">
-        <v>12.6</v>
+        <v>46.4</v>
       </c>
       <c r="H30">
-        <v>-14</v>
+        <v>24.7</v>
       </c>
       <c r="I30">
-        <v>33</v>
+        <v>61.9</v>
       </c>
       <c r="J30" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="K30">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>72</v>
       </c>
@@ -8199,25 +8320,19 @@
         <v>72</v>
       </c>
       <c r="C31" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="D31" t="s">
         <v>53</v>
       </c>
-      <c r="G31">
-        <v>-7.9</v>
-      </c>
-      <c r="H31">
-        <v>-84</v>
-      </c>
-      <c r="I31">
-        <v>37</v>
-      </c>
-      <c r="J31" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E31">
+        <v>758</v>
+      </c>
+      <c r="F31">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>72</v>
       </c>
@@ -8228,16 +8343,22 @@
         <v>52</v>
       </c>
       <c r="D32" t="s">
-        <v>11</v>
-      </c>
-      <c r="E32">
-        <v>509.94489548395501</v>
-      </c>
-      <c r="F32">
-        <v>310.94578768440601</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+      <c r="G32">
+        <v>12.6</v>
+      </c>
+      <c r="H32">
+        <v>-14</v>
+      </c>
+      <c r="I32">
+        <v>33</v>
+      </c>
+      <c r="J32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>72</v>
       </c>
@@ -8248,41 +8369,514 @@
         <v>52</v>
       </c>
       <c r="D33" t="s">
+        <v>53</v>
+      </c>
+      <c r="G33">
+        <v>-7.9</v>
+      </c>
+      <c r="H33">
+        <v>-84</v>
+      </c>
+      <c r="I33">
+        <v>37</v>
+      </c>
+      <c r="J33" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34">
+        <v>509.94489548395501</v>
+      </c>
+      <c r="F34">
+        <v>310.94578768440601</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" t="s">
         <v>10</v>
       </c>
-      <c r="E33">
+      <c r="E35">
         <v>669.92557424909899</v>
       </c>
-      <c r="F33">
+      <c r="F35">
         <v>223.99187806601799</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" t="str">
-        <f>A33</f>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A36" t="str">
+        <f>A35</f>
         <v>Novavax</v>
       </c>
-      <c r="B34" t="str">
-        <f>B33</f>
+      <c r="B36" t="str">
+        <f>B35</f>
         <v>Novavax</v>
       </c>
-      <c r="C34" t="str">
-        <f>C33</f>
+      <c r="C36" t="str">
+        <f>C35</f>
         <v>Elderly</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D36" t="s">
         <v>53</v>
       </c>
-      <c r="E34">
-        <f>GEOMEAN(E32:E33)</f>
+      <c r="E36">
+        <f>GEOMEAN(E34:E35)</f>
         <v>584.48706310959983</v>
       </c>
-      <c r="F34">
-        <f>GEOMEAN(F32:F33)</f>
+      <c r="F36">
+        <f>GEOMEAN(F34:F35)</f>
         <v>263.9115968655932</v>
       </c>
     </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>86</v>
+      </c>
+      <c r="B37" t="s">
+        <v>90</v>
+      </c>
+      <c r="C37" t="s">
+        <v>52</v>
+      </c>
+      <c r="D37" t="s">
+        <v>53</v>
+      </c>
+      <c r="G37">
+        <v>83.7</v>
+      </c>
+      <c r="H37">
+        <v>66</v>
+      </c>
+      <c r="I37">
+        <v>92.2</v>
+      </c>
+      <c r="J37" t="s">
+        <v>55</v>
+      </c>
+      <c r="K37">
+        <v>112</v>
+      </c>
+      <c r="L37" t="s">
+        <v>81</v>
+      </c>
+      <c r="M37" t="s">
+        <v>88</v>
+      </c>
+      <c r="N37" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>86</v>
+      </c>
+      <c r="B38" t="s">
+        <v>90</v>
+      </c>
+      <c r="C38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D38" t="s">
+        <v>53</v>
+      </c>
+      <c r="G38">
+        <v>82.4</v>
+      </c>
+      <c r="H38">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="I38">
+        <v>95.3</v>
+      </c>
+      <c r="J38" t="s">
+        <v>62</v>
+      </c>
+      <c r="K38">
+        <v>112</v>
+      </c>
+      <c r="L38" t="s">
+        <v>81</v>
+      </c>
+      <c r="M38" t="s">
+        <v>87</v>
+      </c>
+      <c r="N38" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>86</v>
+      </c>
+      <c r="B39" t="s">
+        <v>90</v>
+      </c>
+      <c r="C39" t="s">
+        <v>52</v>
+      </c>
+      <c r="D39" t="s">
+        <v>53</v>
+      </c>
+      <c r="G39">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="H39">
+        <v>50.9</v>
+      </c>
+      <c r="I39">
+        <v>79.7</v>
+      </c>
+      <c r="J39" t="s">
+        <v>19</v>
+      </c>
+      <c r="K39">
+        <v>112</v>
+      </c>
+      <c r="L39" t="s">
+        <v>81</v>
+      </c>
+      <c r="M39" t="s">
+        <v>89</v>
+      </c>
+      <c r="N39" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>86</v>
+      </c>
+      <c r="B40" t="s">
+        <v>90</v>
+      </c>
+      <c r="C40" t="s">
+        <v>52</v>
+      </c>
+      <c r="D40" t="s">
+        <v>10</v>
+      </c>
+      <c r="G40">
+        <v>91.7</v>
+      </c>
+      <c r="H40">
+        <v>73</v>
+      </c>
+      <c r="I40">
+        <v>97.4</v>
+      </c>
+      <c r="J40" t="s">
+        <v>55</v>
+      </c>
+      <c r="K40">
+        <v>112</v>
+      </c>
+      <c r="L40" t="s">
+        <v>81</v>
+      </c>
+      <c r="M40" t="s">
+        <v>88</v>
+      </c>
+      <c r="N40" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>86</v>
+      </c>
+      <c r="B41" t="s">
+        <v>90</v>
+      </c>
+      <c r="C41" t="s">
+        <v>52</v>
+      </c>
+      <c r="D41" t="s">
+        <v>10</v>
+      </c>
+      <c r="G41">
+        <v>90</v>
+      </c>
+      <c r="H41">
+        <v>22</v>
+      </c>
+      <c r="I41">
+        <v>98.7</v>
+      </c>
+      <c r="J41" t="s">
+        <v>62</v>
+      </c>
+      <c r="K41">
+        <v>112</v>
+      </c>
+      <c r="L41" t="s">
+        <v>81</v>
+      </c>
+      <c r="M41" t="s">
+        <v>87</v>
+      </c>
+      <c r="N41" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>86</v>
+      </c>
+      <c r="B42" t="s">
+        <v>90</v>
+      </c>
+      <c r="C42" t="s">
+        <v>52</v>
+      </c>
+      <c r="D42" t="s">
+        <v>11</v>
+      </c>
+      <c r="G42">
+        <v>68.5</v>
+      </c>
+      <c r="H42">
+        <v>21.1</v>
+      </c>
+      <c r="I42">
+        <v>87.4</v>
+      </c>
+      <c r="J42" t="s">
+        <v>55</v>
+      </c>
+      <c r="K42">
+        <v>112</v>
+      </c>
+      <c r="L42" t="s">
+        <v>81</v>
+      </c>
+      <c r="M42" t="s">
+        <v>88</v>
+      </c>
+      <c r="N42" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>86</v>
+      </c>
+      <c r="B43" t="s">
+        <v>90</v>
+      </c>
+      <c r="C43" t="s">
+        <v>52</v>
+      </c>
+      <c r="D43" t="s">
+        <v>11</v>
+      </c>
+      <c r="G43">
+        <v>71.5</v>
+      </c>
+      <c r="H43">
+        <v>-37</v>
+      </c>
+      <c r="I43">
+        <v>94.1</v>
+      </c>
+      <c r="J43" t="s">
+        <v>62</v>
+      </c>
+      <c r="K43">
+        <v>112</v>
+      </c>
+      <c r="L43" t="s">
+        <v>81</v>
+      </c>
+      <c r="M43" t="s">
+        <v>87</v>
+      </c>
+      <c r="N43" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" t="s">
+        <v>81</v>
+      </c>
+      <c r="C44" t="s">
+        <v>52</v>
+      </c>
+      <c r="D44" t="s">
+        <v>10</v>
+      </c>
+      <c r="E44">
+        <v>8.3023429415730554</v>
+      </c>
+      <c r="F44">
+        <v>0.90097903892662778</v>
+      </c>
+      <c r="L44" t="s">
+        <v>81</v>
+      </c>
+      <c r="N44" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>86</v>
+      </c>
+      <c r="B45" t="s">
+        <v>81</v>
+      </c>
+      <c r="C45" t="s">
+        <v>52</v>
+      </c>
+      <c r="D45" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45">
+        <v>11.392099607392703</v>
+      </c>
+      <c r="F45">
+        <v>1.1491516857651389</v>
+      </c>
+      <c r="L45" t="s">
+        <v>81</v>
+      </c>
+      <c r="N45" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>86</v>
+      </c>
+      <c r="B46" t="s">
+        <v>81</v>
+      </c>
+      <c r="C46" t="s">
+        <v>52</v>
+      </c>
+      <c r="D46" t="s">
+        <v>53</v>
+      </c>
+      <c r="E46">
+        <f>GEOMEAN(E44:E45)</f>
+        <v>9.7252824002768161</v>
+      </c>
+      <c r="F46">
+        <f>GEOMEAN(F44:F45)</f>
+        <v>1.0175271895244811</v>
+      </c>
+      <c r="L46" t="s">
+        <v>81</v>
+      </c>
+      <c r="N46" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>86</v>
+      </c>
+      <c r="B47" t="s">
+        <v>81</v>
+      </c>
+      <c r="C47" t="s">
+        <v>92</v>
+      </c>
+      <c r="D47" t="s">
+        <v>10</v>
+      </c>
+      <c r="E47">
+        <v>14.652591571562276</v>
+      </c>
+      <c r="F47">
+        <v>1.0888620819744395</v>
+      </c>
+      <c r="L47" t="s">
+        <v>81</v>
+      </c>
+      <c r="N47" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>86</v>
+      </c>
+      <c r="B48" t="s">
+        <v>81</v>
+      </c>
+      <c r="C48" t="s">
+        <v>92</v>
+      </c>
+      <c r="D48" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48">
+        <v>20.929300664290945</v>
+      </c>
+      <c r="F48">
+        <v>0.91677793244260819</v>
+      </c>
+      <c r="L48" t="s">
+        <v>81</v>
+      </c>
+      <c r="N48" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>86</v>
+      </c>
+      <c r="B49" t="s">
+        <v>81</v>
+      </c>
+      <c r="C49" t="s">
+        <v>92</v>
+      </c>
+      <c r="D49" t="s">
+        <v>53</v>
+      </c>
+      <c r="E49">
+        <f>GEOMEAN(E47:E48)</f>
+        <v>17.511952904010514</v>
+      </c>
+      <c r="F49">
+        <f>GEOMEAN(F47:F48)</f>
+        <v>0.99912197865309738</v>
+      </c>
+      <c r="L49" t="s">
+        <v>81</v>
+      </c>
+      <c r="N49" t="s">
+        <v>91</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:O48" xr:uid="{87136465-2DAE-EE48-9DCA-BA1E3F450528}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>